<commit_message>
index file for github pages
</commit_message>
<xml_diff>
--- a/Results_RNN_g10_TC.xlsx
+++ b/Results_RNN_g10_TC.xlsx
@@ -380,7 +380,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -518,6 +518,72 @@
         <v>251</v>
       </c>
     </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="B13">
+        <v>0.6510902716008173</v>
+      </c>
+      <c r="C13">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="B14">
+        <v>1.417572166828469</v>
+      </c>
+      <c r="C14">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>0.3408662900188323</v>
+      </c>
+      <c r="B15">
+        <v>0.4124583697988894</v>
+      </c>
+      <c r="C15">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="B16">
+        <v>0.3708246387322489</v>
+      </c>
+      <c r="C16">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>0.3408662900188323</v>
+      </c>
+      <c r="B17">
+        <v>3.521417708659667</v>
+      </c>
+      <c r="C17">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="B18">
+        <v>2.090990100992806</v>
+      </c>
+      <c r="C18">
+        <v>257</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>